<commit_message>
Only provide aggregation mapping and abbreviations in main file SEDOS-structure-all for easier adaption
</commit_message>
<xml_diff>
--- a/sedos_dashboard/media/structures/SEDOS-structure-transport-sector-coupled.xlsx
+++ b/sedos_dashboard/media/structures/SEDOS-structure-transport-sector-coupled.xlsx
@@ -8,18 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ga38hir\git\github\SEDOS_GUI\sedos_dashboard\sedos_dashboard\media\structures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E98803F-F0F9-4CB8-A55F-489AE08E64A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD08622A-604B-44D5-A5B7-E412C617C6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Process_Set" sheetId="5" r:id="rId1"/>
     <sheet name="Helper_Set" sheetId="6" r:id="rId2"/>
-    <sheet name="Abbreviations" sheetId="7" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Abbreviations!$A$1:$B$228</definedName>
-  </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,40 +36,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Unbekannter Autor</author>
-  </authors>
-  <commentList>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{428BD9E4-950A-4951-8A4A-720D9766AB1B}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Gian Müller:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Ich glaube aec und ael könnten zusammengeführt werden
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3136" uniqueCount="1766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2676" uniqueCount="1325">
   <si>
     <t>input</t>
   </si>
@@ -4065,1367 +4029,12 @@
   <si>
     <t>helper_sink_exo_road_const_diesel</t>
   </si>
-  <si>
-    <t>abbreviations</t>
-  </si>
-  <si>
-    <t>meaning</t>
-  </si>
-  <si>
-    <t>a-si</t>
-  </si>
-  <si>
-    <t>amorphous silicon</t>
-  </si>
-  <si>
-    <t>abs</t>
-  </si>
-  <si>
-    <t>absorption</t>
-  </si>
-  <si>
-    <t>ads</t>
-  </si>
-  <si>
-    <t>adsorbtion</t>
-  </si>
-  <si>
-    <t>aec</t>
-  </si>
-  <si>
-    <t>alkaline electrolysis cell</t>
-  </si>
-  <si>
-    <t>agri</t>
-  </si>
-  <si>
-    <t>agriculture</t>
-  </si>
-  <si>
-    <t>aluminabayer</t>
-  </si>
-  <si>
-    <t>alumina bayer</t>
-  </si>
-  <si>
-    <t>aluminium</t>
-  </si>
-  <si>
-    <t>amcr</t>
-  </si>
-  <si>
-    <t>ammonia cracker</t>
-  </si>
-  <si>
-    <t>automobile</t>
-  </si>
-  <si>
-    <t>automobile industry</t>
-  </si>
-  <si>
-    <t>balc</t>
-  </si>
-  <si>
-    <t>balcony</t>
-  </si>
-  <si>
-    <t>batt</t>
-  </si>
-  <si>
-    <t>battery</t>
-  </si>
-  <si>
-    <t>bdys</t>
-  </si>
-  <si>
-    <t>automobile body shop</t>
-  </si>
-  <si>
-    <t>bemu</t>
-  </si>
-  <si>
-    <t>Battery Electric Multiple Units</t>
-  </si>
-  <si>
-    <t>bev</t>
-  </si>
-  <si>
-    <t>battery electric vehicle</t>
-  </si>
-  <si>
-    <t>bfp</t>
-  </si>
-  <si>
-    <t>biofuel production</t>
-  </si>
-  <si>
-    <t>bi</t>
-  </si>
-  <si>
-    <t>bi directional charging</t>
-  </si>
-  <si>
-    <t>biog</t>
-  </si>
-  <si>
-    <t>biomass gassification</t>
-  </si>
-  <si>
-    <t>biom</t>
-  </si>
-  <si>
-    <t>biological methanation</t>
-  </si>
-  <si>
-    <t>blafu</t>
-  </si>
-  <si>
-    <t>blast_furnace</t>
-  </si>
-  <si>
-    <t>blligas</t>
-  </si>
-  <si>
-    <t>black_liqueor_gasification</t>
-  </si>
-  <si>
-    <t>boil</t>
-  </si>
-  <si>
-    <t>boiler</t>
-  </si>
-  <si>
-    <t>btry</t>
-  </si>
-  <si>
-    <t>Automobile battery</t>
-  </si>
-  <si>
-    <t>btx</t>
-  </si>
-  <si>
-    <t>benzene, toluene, Xylene (aromatics)</t>
-  </si>
-  <si>
-    <t>bus</t>
-  </si>
-  <si>
-    <t>car</t>
-  </si>
-  <si>
-    <t>casting</t>
-  </si>
-  <si>
-    <t>casting plant</t>
-  </si>
-  <si>
-    <t>cc</t>
-  </si>
-  <si>
-    <t>combined cycle</t>
-  </si>
-  <si>
-    <t>ccs</t>
-  </si>
-  <si>
-    <t>carbon capture and storage</t>
-  </si>
-  <si>
-    <t>cd</t>
-  </si>
-  <si>
-    <t>condensing</t>
-  </si>
-  <si>
-    <t>cement</t>
-  </si>
-  <si>
-    <t>chemical</t>
-  </si>
-  <si>
-    <t>chemical industry</t>
-  </si>
-  <si>
-    <t>chp</t>
-  </si>
-  <si>
-    <t>combined heat and power</t>
-  </si>
-  <si>
-    <t>cl2</t>
-  </si>
-  <si>
-    <t>chlorine</t>
-  </si>
-  <si>
-    <t>cng</t>
-  </si>
-  <si>
-    <t>compressed natural gas</t>
-  </si>
-  <si>
-    <t>coel</t>
-  </si>
-  <si>
-    <t>co-electrolysis</t>
-  </si>
-  <si>
-    <t>comp</t>
-  </si>
-  <si>
-    <t>compression</t>
-  </si>
-  <si>
-    <t>const</t>
-  </si>
-  <si>
-    <t>construction</t>
-  </si>
-  <si>
-    <t>construction vehicle</t>
-  </si>
-  <si>
-    <t>cont</t>
-  </si>
-  <si>
-    <t>container</t>
-  </si>
-  <si>
-    <t>copper</t>
-  </si>
-  <si>
-    <t>cpv</t>
-  </si>
-  <si>
-    <t>concentrated-PV</t>
-  </si>
-  <si>
-    <t>cts</t>
-  </si>
-  <si>
-    <t>commercial trade &amp; service</t>
-  </si>
-  <si>
-    <t>cv</t>
-  </si>
-  <si>
-    <t>commercial vehicle</t>
-  </si>
-  <si>
-    <t>dac</t>
-  </si>
-  <si>
-    <t>direct air capture</t>
-  </si>
-  <si>
-    <t>daccs</t>
-  </si>
-  <si>
-    <t>direct air carbon capture &amp; storage</t>
-  </si>
-  <si>
-    <t>diaph</t>
-  </si>
-  <si>
-    <t>Chlorine diaphragm production process</t>
-  </si>
-  <si>
-    <t>dirred</t>
-  </si>
-  <si>
-    <t>direct reduction</t>
-  </si>
-  <si>
-    <t>eb</t>
-  </si>
-  <si>
-    <t>electrode boiler</t>
-  </si>
-  <si>
-    <t>echem</t>
-  </si>
-  <si>
-    <t>electro-chemical process</t>
-  </si>
-  <si>
-    <t>ecrac</t>
-  </si>
-  <si>
-    <t>electro cracking</t>
-  </si>
-  <si>
-    <t>eem</t>
-  </si>
-  <si>
-    <t>european electricity market</t>
-  </si>
-  <si>
-    <t>elefu</t>
-  </si>
-  <si>
-    <t>electric furnace</t>
-  </si>
-  <si>
-    <t>emi</t>
-  </si>
-  <si>
-    <t>emissions</t>
-  </si>
-  <si>
-    <t>envir</t>
-  </si>
-  <si>
-    <t>environmental</t>
-  </si>
-  <si>
-    <t>et</t>
-  </si>
-  <si>
-    <t>electrode</t>
-  </si>
-  <si>
-    <t>europ</t>
-  </si>
-  <si>
-    <t>european</t>
-  </si>
-  <si>
-    <t>ev</t>
-  </si>
-  <si>
-    <t>electric vehicle</t>
-  </si>
-  <si>
-    <t>exo</t>
-  </si>
-  <si>
-    <t>exogenous demand</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <charset val="1"/>
-      </rPr>
-      <t>f</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <charset val="1"/>
-      </rPr>
-      <t>uel spefic emission</t>
-    </r>
-  </si>
-  <si>
-    <t>faca</t>
-  </si>
-  <si>
-    <t>facade</t>
-  </si>
-  <si>
-    <t>fasmbl</t>
-  </si>
-  <si>
-    <t>automobile final assembly</t>
-  </si>
-  <si>
-    <t>fb</t>
-  </si>
-  <si>
-    <t>fixed bottom</t>
-  </si>
-  <si>
-    <t>fc</t>
-  </si>
-  <si>
-    <t>fuelcell</t>
-  </si>
-  <si>
-    <t>fcev</t>
-  </si>
-  <si>
-    <t>fuel cell electric vehicle</t>
-  </si>
-  <si>
-    <t>fibe</t>
-  </si>
-  <si>
-    <t>fiber</t>
-  </si>
-  <si>
-    <t>finish</t>
-  </si>
-  <si>
-    <t>finishing process</t>
-  </si>
-  <si>
-    <t>fis</t>
-  </si>
-  <si>
-    <t>fission</t>
-  </si>
-  <si>
-    <t>fix-conversion</t>
-  </si>
-  <si>
-    <t>hybrid</t>
-  </si>
-  <si>
-    <t>fl</t>
-  </si>
-  <si>
-    <t>floating</t>
-  </si>
-  <si>
-    <t>flat</t>
-  </si>
-  <si>
-    <t>flex</t>
-  </si>
-  <si>
-    <t>flexible charging by grid operator</t>
-  </si>
-  <si>
-    <t>frei</t>
-  </si>
-  <si>
-    <t>freight</t>
-  </si>
-  <si>
-    <t>ft</t>
-  </si>
-  <si>
-    <t>fischer-tropsch process</t>
-  </si>
-  <si>
-    <t>fulle</t>
-  </si>
-  <si>
-    <t>fullelectric</t>
-  </si>
-  <si>
-    <t>fus</t>
-  </si>
-  <si>
-    <t>fusion</t>
-  </si>
-  <si>
-    <t>g2v</t>
-  </si>
-  <si>
-    <t>grid to vehicle</t>
-  </si>
-  <si>
-    <t>geoth</t>
-  </si>
-  <si>
-    <t>geothermal</t>
-  </si>
-  <si>
-    <t>glass</t>
-  </si>
-  <si>
-    <t>gliq</t>
-  </si>
-  <si>
-    <t>gas liquiefier</t>
-  </si>
-  <si>
-    <t>gm</t>
-  </si>
-  <si>
-    <t>ground mounted</t>
-  </si>
-  <si>
-    <t>gro</t>
-  </si>
-  <si>
-    <t>ground</t>
-  </si>
-  <si>
-    <t>gt</t>
-  </si>
-  <si>
-    <t>gas turbine</t>
-  </si>
-  <si>
-    <t>ha</t>
-  </si>
-  <si>
-    <t>horizontal axis</t>
-  </si>
-  <si>
-    <t>hb</t>
-  </si>
-  <si>
-    <t>haber-bosch process</t>
-  </si>
-  <si>
-    <t>hcar</t>
-  </si>
-  <si>
-    <t>heavy car</t>
-  </si>
-  <si>
-    <t>hchem</t>
-  </si>
-  <si>
-    <t>high quality paper chemical pulp extraction</t>
-  </si>
-  <si>
-    <t>hcv</t>
-  </si>
-  <si>
-    <t>heavy commercial vehicle</t>
-  </si>
-  <si>
-    <t>hea</t>
-  </si>
-  <si>
-    <t>heat</t>
-  </si>
-  <si>
-    <t>hfo</t>
-  </si>
-  <si>
-    <t>heavy fuel oil</t>
-  </si>
-  <si>
-    <t>hh</t>
-  </si>
-  <si>
-    <t>households</t>
-  </si>
-  <si>
-    <t>hpl</t>
-  </si>
-  <si>
-    <t>heatpump large</t>
-  </si>
-  <si>
-    <t>hps</t>
-  </si>
-  <si>
-    <t>heatpump small</t>
-  </si>
-  <si>
-    <t>ht</t>
-  </si>
-  <si>
-    <t>high-temperature</t>
-  </si>
-  <si>
-    <t>hth</t>
-  </si>
-  <si>
-    <t>high temperature heat</t>
-  </si>
-  <si>
-    <t>htruck</t>
-  </si>
-  <si>
-    <t>heavy truck</t>
-  </si>
-  <si>
-    <t>hvc</t>
-  </si>
-  <si>
-    <t>high value chemicals (olefins and aromatics)</t>
-  </si>
-  <si>
-    <t>hvlt</t>
-  </si>
-  <si>
-    <t>automobile hvac and light</t>
-  </si>
-  <si>
-    <t>hyb</t>
-  </si>
-  <si>
-    <t>hybrid electric vehicle</t>
-  </si>
-  <si>
-    <t>hyddri</t>
-  </si>
-  <si>
-    <t>hydrogen direct reduction</t>
-  </si>
-  <si>
-    <t>hydr</t>
-  </si>
-  <si>
-    <t>hydro</t>
-  </si>
-  <si>
-    <t>ic</t>
-  </si>
-  <si>
-    <t>internal combustion</t>
-  </si>
-  <si>
-    <t>icev</t>
-  </si>
-  <si>
-    <t>internal combustion engine vehicle</t>
-  </si>
-  <si>
-    <t>iip</t>
-  </si>
-  <si>
-    <t>industrial intermediate product</t>
-  </si>
-  <si>
-    <t>ind</t>
-  </si>
-  <si>
-    <t>industry</t>
-  </si>
-  <si>
-    <t>infl</t>
-  </si>
-  <si>
-    <t>inflexible charging, controlled by vehicle owner</t>
-  </si>
-  <si>
-    <t>inter</t>
-  </si>
-  <si>
-    <t>international</t>
-  </si>
-  <si>
-    <t>intg</t>
-  </si>
-  <si>
-    <t>integrated painting process</t>
-  </si>
-  <si>
-    <t>lcar</t>
-  </si>
-  <si>
-    <t>light car</t>
-  </si>
-  <si>
-    <t>lchem</t>
-  </si>
-  <si>
-    <t>low quality paper chemical pulp extraction</t>
-  </si>
-  <si>
-    <t>lcv</t>
-  </si>
-  <si>
-    <t>light commercial vehicle</t>
-  </si>
-  <si>
-    <t>lmech</t>
-  </si>
-  <si>
-    <t>low quality paper mechanical pulp extraction</t>
-  </si>
-  <si>
-    <t>lng</t>
-  </si>
-  <si>
-    <t>liquefied natural gas</t>
-  </si>
-  <si>
-    <t>lohc</t>
-  </si>
-  <si>
-    <t>liquid organic hydrogen carrier</t>
-  </si>
-  <si>
-    <t>lpg</t>
-  </si>
-  <si>
-    <t>liquefied petroleum gas</t>
-  </si>
-  <si>
-    <t>ls</t>
-  </si>
-  <si>
-    <t>large-scale</t>
-  </si>
-  <si>
-    <t>lt</t>
-  </si>
-  <si>
-    <t>low-temperature</t>
-  </si>
-  <si>
-    <t>lth</t>
-  </si>
-  <si>
-    <t>low temperature heat</t>
-  </si>
-  <si>
-    <t>ltruck</t>
-  </si>
-  <si>
-    <t>light truck</t>
-  </si>
-  <si>
-    <t>m-si</t>
-  </si>
-  <si>
-    <t>monocristalline silicon</t>
-  </si>
-  <si>
-    <t>mcar</t>
-  </si>
-  <si>
-    <t>medium sized car</t>
-  </si>
-  <si>
-    <t>mcfc</t>
-  </si>
-  <si>
-    <t>molten carbon fuel cell</t>
-  </si>
-  <si>
-    <t>mche</t>
-  </si>
-  <si>
-    <t>methanisation chemical</t>
-  </si>
-  <si>
-    <t>mcmp</t>
-  </si>
-  <si>
-    <t>automobile material handling and compressed air</t>
-  </si>
-  <si>
-    <t>mdrive</t>
-  </si>
-  <si>
-    <t>machine drive process</t>
-  </si>
-  <si>
-    <t>me1</t>
-  </si>
-  <si>
-    <t>multi apartment building  older than 1979</t>
-  </si>
-  <si>
-    <t>me2</t>
-  </si>
-  <si>
-    <t>multi apartment building 1979-2001</t>
-  </si>
-  <si>
-    <t>me3</t>
-  </si>
-  <si>
-    <t>multi apartment building 2001-2015</t>
-  </si>
-  <si>
-    <t>memb</t>
-  </si>
-  <si>
-    <t>Standard Chlorine membrane production process</t>
-  </si>
-  <si>
-    <t>membcc</t>
-  </si>
-  <si>
-    <t>Advanced Membrane Production zero Cap Catalytic Coat</t>
-  </si>
-  <si>
-    <t>memboxy</t>
-  </si>
-  <si>
-    <t>Membrane Cells with oxygen consuming cathodes</t>
-  </si>
-  <si>
-    <t>meoh</t>
-  </si>
-  <si>
-    <t>methanol</t>
-  </si>
-  <si>
-    <t>mhydr</t>
-  </si>
-  <si>
-    <t>methanol synthesis from CO2 hydrogenation</t>
-  </si>
-  <si>
-    <t>mn1</t>
-  </si>
-  <si>
-    <t>multi apartment building new</t>
-  </si>
-  <si>
-    <t>motorc</t>
-  </si>
-  <si>
-    <t>motorcycle</t>
-  </si>
-  <si>
-    <t>mpyr</t>
-  </si>
-  <si>
-    <t>methane pyrolysis</t>
-  </si>
-  <si>
-    <t>msyn</t>
-  </si>
-  <si>
-    <t>methanol synthesis</t>
-  </si>
-  <si>
-    <t>msynth</t>
-  </si>
-  <si>
-    <t>methanol synthesis from fossil feedstockl based H2/syngas</t>
-  </si>
-  <si>
-    <t>mta</t>
-  </si>
-  <si>
-    <t>methanol-to-aromatics</t>
-  </si>
-  <si>
-    <t>mtg</t>
-  </si>
-  <si>
-    <t>Methanol-to-gasoline </t>
-  </si>
-  <si>
-    <t>mtk</t>
-  </si>
-  <si>
-    <t>Methanol-to-kerosene</t>
-  </si>
-  <si>
-    <t>mto</t>
-  </si>
-  <si>
-    <t>methanol-to-olefin</t>
-  </si>
-  <si>
-    <t>mtoa</t>
-  </si>
-  <si>
-    <t>methanol to olefins/aromatics</t>
-  </si>
-  <si>
-    <t>mtruck</t>
-  </si>
-  <si>
-    <t>mid sized truck</t>
-  </si>
-  <si>
-    <t>natgas</t>
-  </si>
-  <si>
-    <t>natural gas</t>
-  </si>
-  <si>
-    <t>natio</t>
-  </si>
-  <si>
-    <t>national</t>
-  </si>
-  <si>
-    <t>near</t>
-  </si>
-  <si>
-    <t>nearshore</t>
-  </si>
-  <si>
-    <t>nh3</t>
-  </si>
-  <si>
-    <t>ammonia</t>
-  </si>
-  <si>
-    <t>novel</t>
-  </si>
-  <si>
-    <t>novelfinish</t>
-  </si>
-  <si>
-    <t>finishing process for novel cements</t>
-  </si>
-  <si>
-    <t>ocm</t>
-  </si>
-  <si>
-    <t>oxidative coupling of methan</t>
-  </si>
-  <si>
-    <t>oev</t>
-  </si>
-  <si>
-    <t>overhead electric vehicle</t>
-  </si>
-  <si>
-    <t>off</t>
-  </si>
-  <si>
-    <t>offshore</t>
-  </si>
-  <si>
-    <t>olefins</t>
-  </si>
-  <si>
-    <t>olefins- Ethylen, Propylen, Buten und Butadien</t>
-  </si>
-  <si>
-    <t>on</t>
-  </si>
-  <si>
-    <t>onshore</t>
-  </si>
-  <si>
-    <t>orc</t>
-  </si>
-  <si>
-    <t>organic rankine cycle</t>
-  </si>
-  <si>
-    <t>oref</t>
-  </si>
-  <si>
-    <t>oil refinery</t>
-  </si>
-  <si>
-    <t>oxyf</t>
-  </si>
-  <si>
-    <t>oxyfuel</t>
-  </si>
-  <si>
-    <t>oxyfu</t>
-  </si>
-  <si>
-    <t>oxygen furnace</t>
-  </si>
-  <si>
-    <t>oxyh</t>
-  </si>
-  <si>
-    <t>oxyhybrid</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <charset val="1"/>
-      </rPr>
-      <t>p</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <charset val="1"/>
-      </rPr>
-      <t>rocess specific emission</t>
-    </r>
-  </si>
-  <si>
-    <t>p-si</t>
-  </si>
-  <si>
-    <t>polycristalline silicon</t>
-  </si>
-  <si>
-    <t>paper</t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>passenger</t>
-  </si>
-  <si>
-    <t>pc</t>
-  </si>
-  <si>
-    <t>passenger car</t>
-  </si>
-  <si>
-    <t>pellet</t>
-  </si>
-  <si>
-    <t>pemec</t>
-  </si>
-  <si>
-    <t>proton exchange membrane electrolysis cell</t>
-  </si>
-  <si>
-    <t>pemfc</t>
-  </si>
-  <si>
-    <t>proton exchange membrane fuel cell</t>
-  </si>
-  <si>
-    <t>phev</t>
-  </si>
-  <si>
-    <t>plug-in hybrid electric vehicle</t>
-  </si>
-  <si>
-    <t>pnts</t>
-  </si>
-  <si>
-    <t>automobile paint shop</t>
-  </si>
-  <si>
-    <t>pond</t>
-  </si>
-  <si>
-    <t>pondage</t>
-  </si>
-  <si>
-    <t>pow</t>
-  </si>
-  <si>
-    <t>power</t>
-  </si>
-  <si>
-    <t>pox</t>
-  </si>
-  <si>
-    <t>partial oxydization</t>
-  </si>
-  <si>
-    <t>pri</t>
-  </si>
-  <si>
-    <t>primary</t>
-  </si>
-  <si>
-    <t>proc</t>
-  </si>
-  <si>
-    <t>prtp</t>
-  </si>
-  <si>
-    <t>automobile parts production</t>
-  </si>
-  <si>
-    <t>psa</t>
-  </si>
-  <si>
-    <t>pressure swing adsorption</t>
-  </si>
-  <si>
-    <t>pv</t>
-  </si>
-  <si>
-    <t>photovoltaic</t>
-  </si>
-  <si>
-    <t>re1</t>
-  </si>
-  <si>
-    <t>rural existing building older than 1979</t>
-  </si>
-  <si>
-    <t>re2</t>
-  </si>
-  <si>
-    <t>rural existing building 1979-2001</t>
-  </si>
-  <si>
-    <t>re3</t>
-  </si>
-  <si>
-    <t>rural existing building 2001-20015</t>
-  </si>
-  <si>
-    <t>recu</t>
-  </si>
-  <si>
-    <t>recuperative</t>
-  </si>
-  <si>
-    <t>rege</t>
-  </si>
-  <si>
-    <t>regenerative</t>
-  </si>
-  <si>
-    <t>rk</t>
-  </si>
-  <si>
-    <t>rotary kiln</t>
-  </si>
-  <si>
-    <t>rn1</t>
-  </si>
-  <si>
-    <t>rural building new</t>
-  </si>
-  <si>
-    <t>roof</t>
-  </si>
-  <si>
-    <t>rooftop</t>
-  </si>
-  <si>
-    <t>ror</t>
-  </si>
-  <si>
-    <t>run-of-river</t>
-  </si>
-  <si>
-    <t>rwgs</t>
-  </si>
-  <si>
-    <t>reverse water gas shift</t>
-  </si>
-  <si>
-    <t>sabm</t>
-  </si>
-  <si>
-    <t>sabatier methanation</t>
-  </si>
-  <si>
-    <t>scrac</t>
-  </si>
-  <si>
-    <t>steam cracking</t>
-  </si>
-  <si>
-    <t>sec</t>
-  </si>
-  <si>
-    <t>secondary</t>
-  </si>
-  <si>
-    <t>sinter</t>
-  </si>
-  <si>
-    <t>soco</t>
-  </si>
-  <si>
-    <t>solar collector</t>
-  </si>
-  <si>
-    <t>soec</t>
-  </si>
-  <si>
-    <t>solid oxide electrolysis cell</t>
-  </si>
-  <si>
-    <t>sofc</t>
-  </si>
-  <si>
-    <t>solid oxide fuel cell</t>
-  </si>
-  <si>
-    <t>spec</t>
-  </si>
-  <si>
-    <t>special</t>
-  </si>
-  <si>
-    <t>sponge</t>
-  </si>
-  <si>
-    <t>sponge iron</t>
-  </si>
-  <si>
-    <t>sr</t>
-  </si>
-  <si>
-    <t>steam methane reformer</t>
-  </si>
-  <si>
-    <t>st</t>
-  </si>
-  <si>
-    <t>steam turbine</t>
-  </si>
-  <si>
-    <t>steam</t>
-  </si>
-  <si>
-    <t>steam engine</t>
-  </si>
-  <si>
-    <t>steel</t>
-  </si>
-  <si>
-    <t>stov</t>
-  </si>
-  <si>
-    <t>stove</t>
-  </si>
-  <si>
-    <t>t1e</t>
-  </si>
-  <si>
-    <t>type 1 existing building</t>
-  </si>
-  <si>
-    <t>t1n</t>
-  </si>
-  <si>
-    <t>type 1 new building</t>
-  </si>
-  <si>
-    <t>t2e</t>
-  </si>
-  <si>
-    <t>type 2 existing building</t>
-  </si>
-  <si>
-    <t>t2n</t>
-  </si>
-  <si>
-    <t>type 2 new building</t>
-  </si>
-  <si>
-    <t>tra</t>
-  </si>
-  <si>
-    <t>transport</t>
-  </si>
-  <si>
-    <t>ue1</t>
-  </si>
-  <si>
-    <t>urban existing building older than 1979</t>
-  </si>
-  <si>
-    <t>ue2</t>
-  </si>
-  <si>
-    <t>urban existing building 1979-2001</t>
-  </si>
-  <si>
-    <t>ue3</t>
-  </si>
-  <si>
-    <t>urban existing building 2001-2015</t>
-  </si>
-  <si>
-    <t>un1</t>
-  </si>
-  <si>
-    <t>urban building new</t>
-  </si>
-  <si>
-    <t>uni</t>
-  </si>
-  <si>
-    <t>uni directional charging</t>
-  </si>
-  <si>
-    <t>util</t>
-  </si>
-  <si>
-    <t>utility</t>
-  </si>
-  <si>
-    <t>v2g</t>
-  </si>
-  <si>
-    <t>vehicle to grid</t>
-  </si>
-  <si>
-    <t>va</t>
-  </si>
-  <si>
-    <t>vertical axis</t>
-  </si>
-  <si>
-    <t>wow</t>
-  </si>
-  <si>
-    <t>wet-on-wet painting process</t>
-  </si>
-  <si>
-    <t>wt</t>
-  </si>
-  <si>
-    <t>wind turbine</t>
-  </si>
-  <si>
-    <t>x2x</t>
-  </si>
-  <si>
-    <t>power-to-X and other conversion</t>
-  </si>
-  <si>
-    <t>prpt</t>
-  </si>
-  <si>
-    <t>Parts Production Process</t>
-  </si>
-  <si>
-    <t>dh</t>
-  </si>
-  <si>
-    <t>district heating</t>
-  </si>
-  <si>
-    <t>elc</t>
-  </si>
-  <si>
-    <t>electricity</t>
-  </si>
-  <si>
-    <t>rfg</t>
-  </si>
-  <si>
-    <t>refinery gas</t>
-  </si>
-  <si>
-    <t>slu</t>
-  </si>
-  <si>
-    <t>sludge</t>
-  </si>
-  <si>
-    <t>smr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">steam methane reforming </t>
-  </si>
-  <si>
-    <t>carbon capture</t>
-  </si>
-  <si>
-    <t>nap</t>
-  </si>
-  <si>
-    <t>naphtha</t>
-  </si>
-  <si>
-    <t>cog</t>
-  </si>
-  <si>
-    <t>coke oven gas</t>
-  </si>
-  <si>
-    <t>ict</t>
-  </si>
-  <si>
-    <t>information and communication technology</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5483,46 +4092,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -5550,24 +4119,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -5581,7 +4137,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -5596,25 +4152,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Default 1" xfId="3" xr:uid="{B7DDC4D9-29C5-4067-862D-08486F9E9D38}"/>
@@ -5921,7 +4458,7 @@
   <dimension ref="A1:C820"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15831,1875 +14368,4 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F7D23B-2871-4F34-9734-810A66E6B4BA}">
-  <sheetPr>
-    <tabColor rgb="FFA5A5A5"/>
-  </sheetPr>
-  <dimension ref="A1:B230"/>
-  <sheetViews>
-    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A231" sqref="A231"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.28515625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="41.28515625" style="12" customWidth="1"/>
-    <col min="3" max="16384" width="9.85546875" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>1325</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>1326</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1327</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1328</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>1329</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1330</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>1331</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1332</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>1333</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>1334</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>1335</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>1336</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
-        <v>1337</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>1338</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>1339</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>1340</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>1341</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>1342</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>1343</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>1344</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>1345</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>1346</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>1347</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>1348</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>1349</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>1350</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>1351</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>1352</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>1353</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>1354</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>1355</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
-        <v>1356</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>1357</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>1358</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>1359</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>1360</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>1361</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>1362</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>1363</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>1364</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>1365</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>1366</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>1367</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>1368</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>1369</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>1370</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>1371</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>1372</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>1372</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>1373</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>1373</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="11" t="s">
-        <v>1374</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>1376</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>1378</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>1379</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>1380</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>1381</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
-        <v>1382</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>1382</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>1383</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>1384</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>1385</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>1386</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>1387</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>1388</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>1389</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>1390</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>1391</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>1393</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>1394</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>1395</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>1396</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="12" t="s">
-        <v>1395</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>1397</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>1398</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>1399</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
-        <v>1398</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>1399</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A42" s="10" t="s">
-        <v>1400</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>1401</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>1402</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>1403</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>1404</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>1405</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>1406</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>1407</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>1408</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>1409</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>1410</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>1411</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>1412</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A49" s="11" t="s">
-        <v>1413</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>1414</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A50" s="11" t="s">
-        <v>1415</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>1416</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>1417</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>1418</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
-        <v>1419</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>1420</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>1421</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>1422</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A54" s="11" t="s">
-        <v>1423</v>
-      </c>
-      <c r="B54" s="11" t="s">
-        <v>1424</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>1425</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>1426</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
-        <v>1427</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>1428</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>1429</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>1430</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>1431</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>1432</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
-        <v>1433</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>1434</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
-        <v>1435</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>1436</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>1437</v>
-      </c>
-      <c r="B61" s="13" t="s">
-        <v>1438</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
-        <v>1439</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>1440</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
-        <v>1441</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>1442</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
-        <v>1443</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>1444</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
-        <v>1445</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>1446</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
-        <v>1447</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>1448</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
-        <v>1449</v>
-      </c>
-      <c r="B67" s="10" t="s">
-        <v>1450</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A68" s="11" t="s">
-        <v>1451</v>
-      </c>
-      <c r="B68" s="11" t="s">
-        <v>1452</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
-        <v>1453</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>1454</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A70" s="2" t="s">
-        <v>1455</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>1456</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
-        <v>1457</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>1458</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A72" s="2" t="s">
-        <v>1459</v>
-      </c>
-      <c r="B72" s="10" t="s">
-        <v>1459</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="12" t="s">
-        <v>1460</v>
-      </c>
-      <c r="B73" s="12" t="s">
-        <v>1461</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
-        <v>1462</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>1463</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A75" s="2" t="s">
-        <v>1464</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>1465</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A76" s="2" t="s">
-        <v>1466</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>1467</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A77" s="2" t="s">
-        <v>1468</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>1469</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="12" t="s">
-        <v>1470</v>
-      </c>
-      <c r="B78" s="12" t="s">
-        <v>1471</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A79" s="2" t="s">
-        <v>1472</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>1473</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A80" s="10" t="s">
-        <v>1474</v>
-      </c>
-      <c r="B80" s="10" t="s">
-        <v>1474</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A81" s="2" t="s">
-        <v>1475</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>1476</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A82" s="2" t="s">
-        <v>1477</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>1478</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A83" s="2" t="s">
-        <v>1479</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>1480</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A84" s="2" t="s">
-        <v>1481</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>1482</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A85" s="2" t="s">
-        <v>1483</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>1484</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A86" s="2" t="s">
-        <v>1485</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>1486</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A87" s="2" t="s">
-        <v>1487</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>1488</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A88" s="11" t="s">
-        <v>1489</v>
-      </c>
-      <c r="B88" s="11" t="s">
-        <v>1490</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A89" s="11" t="s">
-        <v>1491</v>
-      </c>
-      <c r="B89" s="11" t="s">
-        <v>1492</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A90" s="2" t="s">
-        <v>1493</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>1494</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A91" s="2" t="s">
-        <v>1495</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>1496</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A92" s="2" t="s">
-        <v>1497</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>1498</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A93" s="2" t="s">
-        <v>1499</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A94" s="2" t="s">
-        <v>1501</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>1502</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A95" s="2" t="s">
-        <v>1503</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>1504</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A96" s="2" t="s">
-        <v>1505</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>1506</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A97" s="2" t="s">
-        <v>1507</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>1508</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A98" s="2" t="s">
-        <v>1509</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>1510</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A99" s="2" t="s">
-        <v>1511</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>1512</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="12" t="s">
-        <v>1513</v>
-      </c>
-      <c r="B100" s="12" t="s">
-        <v>1514</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A101" s="11" t="s">
-        <v>1515</v>
-      </c>
-      <c r="B101" s="11" t="s">
-        <v>1516</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A102" s="2" t="s">
-        <v>1517</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>1518</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A103" s="2" t="s">
-        <v>1519</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>1520</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A104" s="2" t="s">
-        <v>1521</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>1522</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A105" s="2" t="s">
-        <v>1523</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>1524</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A106" s="2" t="s">
-        <v>1525</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="12" t="s">
-        <v>1527</v>
-      </c>
-      <c r="B107" s="12" t="s">
-        <v>1528</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A108" s="2" t="s">
-        <v>1529</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>1530</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A109" s="2" t="s">
-        <v>1531</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>1532</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A110" s="2" t="s">
-        <v>1533</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>1534</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A111" s="11" t="s">
-        <v>1535</v>
-      </c>
-      <c r="B111" s="11" t="s">
-        <v>1536</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A112" s="11" t="s">
-        <v>1537</v>
-      </c>
-      <c r="B112" s="11" t="s">
-        <v>1538</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A113" s="11" t="s">
-        <v>1539</v>
-      </c>
-      <c r="B113" s="11" t="s">
-        <v>1540</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A114" s="11" t="s">
-        <v>1541</v>
-      </c>
-      <c r="B114" s="11" t="s">
-        <v>1542</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A115" s="11" t="s">
-        <v>1543</v>
-      </c>
-      <c r="B115" s="11" t="s">
-        <v>1544</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A116" s="11" t="s">
-        <v>1545</v>
-      </c>
-      <c r="B116" s="11" t="s">
-        <v>1546</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A117" s="11" t="s">
-        <v>1547</v>
-      </c>
-      <c r="B117" s="11" t="s">
-        <v>1548</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A118" s="11" t="s">
-        <v>1549</v>
-      </c>
-      <c r="B118" s="11" t="s">
-        <v>1550</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A119" s="2" t="s">
-        <v>1551</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>1552</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A120" s="2" t="s">
-        <v>1553</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>1554</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A121" s="2" t="s">
-        <v>1555</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>1556</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A122" s="2" t="s">
-        <v>1557</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>1558</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A123" s="2" t="s">
-        <v>1559</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>1560</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A124" s="2" t="s">
-        <v>1561</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>1562</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A125" s="2" t="s">
-        <v>1563</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>1564</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A126" s="2" t="s">
-        <v>1565</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>1566</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A127" s="2" t="s">
-        <v>1567</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>1568</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A128" s="2" t="s">
-        <v>1569</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>1570</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A129" s="2" t="s">
-        <v>1571</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>1572</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A130" s="2" t="s">
-        <v>1573</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>1574</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A131" s="14" t="s">
-        <v>1575</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>1576</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A132" s="14" t="s">
-        <v>1577</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>1578</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A133" s="2" t="s">
-        <v>1579</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A134" s="2" t="s">
-        <v>1581</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>1582</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A135" s="2" t="s">
-        <v>1583</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>1584</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A136" s="2" t="s">
-        <v>1585</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>1586</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A137" s="2" t="s">
-        <v>1587</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A138" s="2" t="s">
-        <v>1589</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>1590</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A139" s="2" t="s">
-        <v>1591</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>1592</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A140" s="2" t="s">
-        <v>1593</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>1594</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A141" s="2" t="s">
-        <v>1595</v>
-      </c>
-      <c r="B141" s="11" t="s">
-        <v>1596</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A142" s="2" t="s">
-        <v>1597</v>
-      </c>
-      <c r="B142" s="11" t="s">
-        <v>1598</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A143" s="2" t="s">
-        <v>1599</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A144" s="2" t="s">
-        <v>1601</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>1602</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="12" t="s">
-        <v>1603</v>
-      </c>
-      <c r="B145" s="12" t="s">
-        <v>1604</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A146" s="2" t="s">
-        <v>1605</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>1606</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A147" s="2" t="s">
-        <v>1607</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>1608</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A148" s="2" t="s">
-        <v>1609</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>1610</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A149" s="2" t="s">
-        <v>1611</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>1612</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A150" s="11" t="s">
-        <v>1613</v>
-      </c>
-      <c r="B150" s="11" t="s">
-        <v>1613</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A151" s="11" t="s">
-        <v>1614</v>
-      </c>
-      <c r="B151" s="11" t="s">
-        <v>1615</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A152" s="2" t="s">
-        <v>1616</v>
-      </c>
-      <c r="B152" s="2" t="s">
-        <v>1617</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A153" s="2" t="s">
-        <v>1618</v>
-      </c>
-      <c r="B153" s="2" t="s">
-        <v>1619</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A154" s="2" t="s">
-        <v>1620</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>1621</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A155" s="2" t="s">
-        <v>1622</v>
-      </c>
-      <c r="B155" s="2" t="s">
-        <v>1623</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A156" s="2" t="s">
-        <v>1624</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>1625</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A157" s="2" t="s">
-        <v>1626</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>1627</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A158" s="2" t="s">
-        <v>1628</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>1629</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A159" s="2" t="s">
-        <v>1630</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>1631</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A160" s="11" t="s">
-        <v>1632</v>
-      </c>
-      <c r="B160" s="11" t="s">
-        <v>1633</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A161" s="2" t="s">
-        <v>1634</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>1635</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A162" s="2" t="s">
-        <v>1636</v>
-      </c>
-      <c r="B162" s="13" t="s">
-        <v>1637</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A163" s="2" t="s">
-        <v>1638</v>
-      </c>
-      <c r="B163" s="2" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A164" s="10" t="s">
-        <v>1640</v>
-      </c>
-      <c r="B164" s="10" t="s">
-        <v>1640</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A165" s="2" t="s">
-        <v>1641</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>1642</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A166" s="11" t="s">
-        <v>1643</v>
-      </c>
-      <c r="B166" s="11" t="s">
-        <v>1644</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A167" s="11" t="s">
-        <v>1645</v>
-      </c>
-      <c r="B167" s="11" t="s">
-        <v>1645</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A168" s="2" t="s">
-        <v>1646</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>1647</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A169" s="2" t="s">
-        <v>1648</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>1649</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A170" s="2" t="s">
-        <v>1650</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>1651</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A171" s="2" t="s">
-        <v>1652</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>1653</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A172" s="2" t="s">
-        <v>1654</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>1655</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A173" s="2" t="s">
-        <v>1656</v>
-      </c>
-      <c r="B173" s="2" t="s">
-        <v>1657</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A174" s="2" t="s">
-        <v>1658</v>
-      </c>
-      <c r="B174" s="2" t="s">
-        <v>1659</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A175" s="2" t="s">
-        <v>1660</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>1661</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A176" s="15" t="s">
-        <v>1662</v>
-      </c>
-      <c r="B176" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A177" s="2" t="s">
-        <v>1663</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>1664</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A178" s="2" t="s">
-        <v>1665</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>1666</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A179" s="2" t="s">
-        <v>1667</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>1668</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A180" s="2" t="s">
-        <v>1669</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>1670</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A181" s="2" t="s">
-        <v>1671</v>
-      </c>
-      <c r="B181" s="2" t="s">
-        <v>1672</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A182" s="2" t="s">
-        <v>1673</v>
-      </c>
-      <c r="B182" s="2" t="s">
-        <v>1674</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A183" s="2" t="s">
-        <v>1675</v>
-      </c>
-      <c r="B183" s="2" t="s">
-        <v>1676</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A184" s="2" t="s">
-        <v>1677</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>1678</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A185" s="2" t="s">
-        <v>1679</v>
-      </c>
-      <c r="B185" s="2" t="s">
-        <v>1680</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A186" s="2" t="s">
-        <v>1681</v>
-      </c>
-      <c r="B186" s="2" t="s">
-        <v>1682</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A187" s="2" t="s">
-        <v>1683</v>
-      </c>
-      <c r="B187" s="2" t="s">
-        <v>1684</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A188" s="2" t="s">
-        <v>1685</v>
-      </c>
-      <c r="B188" s="2" t="s">
-        <v>1686</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A189" s="2" t="s">
-        <v>1687</v>
-      </c>
-      <c r="B189" s="2" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A190" s="2" t="s">
-        <v>1689</v>
-      </c>
-      <c r="B190" s="2" t="s">
-        <v>1690</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A191" s="2" t="s">
-        <v>1691</v>
-      </c>
-      <c r="B191" s="2" t="s">
-        <v>1692</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A192" s="2" t="s">
-        <v>1693</v>
-      </c>
-      <c r="B192" s="2" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A193" s="2" t="s">
-        <v>1693</v>
-      </c>
-      <c r="B193" s="2" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A194" s="11" t="s">
-        <v>1695</v>
-      </c>
-      <c r="B194" s="11" t="s">
-        <v>1695</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A195" s="2" t="s">
-        <v>1696</v>
-      </c>
-      <c r="B195" s="2" t="s">
-        <v>1697</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A196" s="2" t="s">
-        <v>1698</v>
-      </c>
-      <c r="B196" s="2" t="s">
-        <v>1699</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A197" s="2" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B197" s="2" t="s">
-        <v>1701</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A198" s="2" t="s">
-        <v>1702</v>
-      </c>
-      <c r="B198" s="2" t="s">
-        <v>1703</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A199" s="11" t="s">
-        <v>1704</v>
-      </c>
-      <c r="B199" s="11" t="s">
-        <v>1705</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A200" s="5" t="s">
-        <v>1706</v>
-      </c>
-      <c r="B200" s="5" t="s">
-        <v>1707</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A201" s="2" t="s">
-        <v>1708</v>
-      </c>
-      <c r="B201" s="2" t="s">
-        <v>1709</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A202" s="12" t="s">
-        <v>1710</v>
-      </c>
-      <c r="B202" s="12" t="s">
-        <v>1711</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A203" s="10" t="s">
-        <v>1712</v>
-      </c>
-      <c r="B203" s="10" t="s">
-        <v>1712</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A204" s="2" t="s">
-        <v>1713</v>
-      </c>
-      <c r="B204" s="2" t="s">
-        <v>1714</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A205" s="2" t="s">
-        <v>1715</v>
-      </c>
-      <c r="B205" s="2" t="s">
-        <v>1716</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A206" s="2" t="s">
-        <v>1717</v>
-      </c>
-      <c r="B206" s="2" t="s">
-        <v>1718</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A207" s="2" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B207" s="2" t="s">
-        <v>1720</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A208" s="2" t="s">
-        <v>1721</v>
-      </c>
-      <c r="B208" s="2" t="s">
-        <v>1722</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A209" s="2" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B209" s="2" t="s">
-        <v>1724</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A210" s="2" t="s">
-        <v>1725</v>
-      </c>
-      <c r="B210" s="2" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A211" s="2" t="s">
-        <v>1727</v>
-      </c>
-      <c r="B211" s="2" t="s">
-        <v>1728</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A212" s="2" t="s">
-        <v>1729</v>
-      </c>
-      <c r="B212" s="2" t="s">
-        <v>1730</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A213" s="2" t="s">
-        <v>1731</v>
-      </c>
-      <c r="B213" s="2" t="s">
-        <v>1732</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A214" s="12" t="s">
-        <v>1733</v>
-      </c>
-      <c r="B214" s="12" t="s">
-        <v>1734</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A215" s="2" t="s">
-        <v>1735</v>
-      </c>
-      <c r="B215" s="2" t="s">
-        <v>1736</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A216" s="12" t="s">
-        <v>1737</v>
-      </c>
-      <c r="B216" s="12" t="s">
-        <v>1738</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A217" s="2" t="s">
-        <v>1739</v>
-      </c>
-      <c r="B217" s="2" t="s">
-        <v>1740</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A218" s="2" t="s">
-        <v>1741</v>
-      </c>
-      <c r="B218" s="2" t="s">
-        <v>1742</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A219" s="2" t="s">
-        <v>1743</v>
-      </c>
-      <c r="B219" s="2" t="s">
-        <v>1744</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A220" s="2" t="s">
-        <v>1745</v>
-      </c>
-      <c r="B220" s="2" t="s">
-        <v>1746</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A221" s="12" t="s">
-        <v>1747</v>
-      </c>
-      <c r="B221" s="12" t="s">
-        <v>1748</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A222" s="12" t="s">
-        <v>1749</v>
-      </c>
-      <c r="B222" s="12" t="s">
-        <v>1750</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A223" s="12" t="s">
-        <v>1751</v>
-      </c>
-      <c r="B223" s="12" t="s">
-        <v>1752</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A224" s="12" t="s">
-        <v>1753</v>
-      </c>
-      <c r="B224" s="12" t="s">
-        <v>1754</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A225" s="12" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B225" s="12" t="s">
-        <v>1756</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A226" s="12" t="s">
-        <v>1757</v>
-      </c>
-      <c r="B226" s="16" t="s">
-        <v>1758</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A227" s="12" t="s">
-        <v>1376</v>
-      </c>
-      <c r="B227" s="12" t="s">
-        <v>1759</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A228" s="12" t="s">
-        <v>1760</v>
-      </c>
-      <c r="B228" s="12" t="s">
-        <v>1761</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A229" s="12" t="s">
-        <v>1762</v>
-      </c>
-      <c r="B229" s="12" t="s">
-        <v>1763</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A230" s="12" t="s">
-        <v>1764</v>
-      </c>
-      <c r="B230" s="12" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B228" xr:uid="{00000000-0009-0000-0000-000007000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B228">
-      <sortCondition ref="A2:A228"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.70069444444444495" right="0.70069444444444495" top="0.75208333333333299" bottom="0.75208333333333299" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>